<commit_message>
fixing an id bug for imbalanced dataset, and regenerating all embeddings, indexes and metrics
</commit_message>
<xml_diff>
--- a/metrics/debug_metrics.xlsx
+++ b/metrics/debug_metrics.xlsx
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.14285714285714285]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [0.2], 10: [0.14285714285714285]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,12 +487,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [0.5]}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -504,12 +504,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [0.5]}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [1.0], 10: [0.5]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [0.25], 10: [0.1111111111111111]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -572,12 +572,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.25], 10: [0.125]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -606,12 +606,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.3333333333333333], 10: [0.2]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -640,12 +640,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -657,12 +657,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -674,12 +674,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -691,12 +691,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -725,12 +725,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -742,12 +742,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,12 +759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -776,12 +776,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -793,12 +793,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,12 +810,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [0.25]}</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -827,12 +827,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -844,12 +844,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,12 +861,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -895,12 +895,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -912,12 +912,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -929,12 +929,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -946,12 +946,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -980,12 +980,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -997,12 +997,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [0.5]}</t>
+          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1031,12 +1031,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.2], 10: [0.1111111111111111]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.3333333333333333], 10: [0.3333333333333333]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1099,12 +1099,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [0.2]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1218,12 +1218,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [0.3333333333333333], 10: [0.125]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1235,12 +1235,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.2], 10: [0.1111111111111111]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1252,12 +1252,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{1: [0.0], 5: [0.5], 10: [0.5]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1286,12 +1286,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [1.0], 10: [1.0]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{1: [1.0], 5: [0.2], 10: [0.1]}</t>
+          <t>{1: [0.0], 5: [0.0], 10: [0.0]}</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">

</xml_diff>